<commit_message>
Se crea un método el cual se encarga de copiar una sola fila del Excel al feature. Además se incluye otro método que se encarga de pasar un rango de filas del excel al feature.
</commit_message>
<xml_diff>
--- a/src/test/resources/Datadriven/Clientes.xlsx
+++ b/src/test/resources/Datadriven/Clientes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dat-bc\BANCOLOMBIA\AUTOMATIZACIONES\SUCURSALES\AW1177001_SUC_Test\Apertura_Cuentas_Ahorros\src\test\resources\Datadriven\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dat-bc\BANCOLOMBIA\AUTOMATIZACIONES\CleanCode\excel-a-feature\src\test\resources\Datadriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>clientType</t>
   </si>
@@ -75,6 +75,24 @@
   </si>
   <si>
     <t>Yepez Camargo</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Camilo Andres</t>
+  </si>
+  <si>
+    <t>Arango Suarez</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Felipe</t>
+  </si>
+  <si>
+    <t>Jaramillo Lopez</t>
   </si>
 </sst>
 </file>
@@ -147,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -155,6 +173,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,7 +561,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,7 +640,39 @@
         <v>16</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6">
+        <v>40</v>
+      </c>
+      <c r="C5" s="7">
+        <v>31941</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="6">
+        <v>12</v>
+      </c>
+      <c r="C6" s="7">
+        <v>322112</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="G6" s="4"/>
     </row>
   </sheetData>

</xml_diff>